<commit_message>
Has the beginnings of an S-Meter. Audio seems worse than before that was added, so I want to check on that. Uploading the image files (even though the PSDR uses them in code form... still, might be handy)
</commit_message>
<xml_diff>
--- a/Hardware/PSDR1_BOM.xlsx
+++ b/Hardware/PSDR1_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="175">
   <si>
     <t>CSM-X7R-100N-10P-25V-0603</t>
   </si>
@@ -297,9 +297,6 @@
     <t>R7,23</t>
   </si>
   <si>
-    <t>C4,5,37,38,12,14,84,85,90,91</t>
-  </si>
-  <si>
     <t>R10,11</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>535-11201-1-ND</t>
   </si>
   <si>
-    <t>AD8130ARZ-ND</t>
-  </si>
-  <si>
     <t>MCP6N11-010E/SN-ND</t>
   </si>
   <si>
@@ -546,7 +540,10 @@
     <t>535-10520-1-ND</t>
   </si>
   <si>
-    <t>&lt;-MISMATCH! :/</t>
+    <t>C4,5,37,38,13,14,84,85,90,91</t>
+  </si>
+  <si>
+    <t>AD8131ARMZ-ND</t>
   </si>
 </sst>
 </file>
@@ -570,7 +567,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,12 +592,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -614,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -626,7 +617,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,10 +913,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A28" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="600" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C28:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -945,16 +935,16 @@
         <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>85</v>
@@ -974,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>1</v>
@@ -991,7 +981,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>10</v>
@@ -999,7 +989,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>173</v>
       </c>
       <c r="B4" s="6">
         <v>10</v>
@@ -1008,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>3</v>
@@ -1016,7 +1006,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="6">
         <v>6</v>
@@ -1025,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>8</v>
@@ -1033,7 +1023,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="6">
         <v>4</v>
@@ -1042,7 +1032,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>15</v>
@@ -1050,7 +1040,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="6">
         <v>5</v>
@@ -1059,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>12</v>
@@ -1067,7 +1057,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="6">
         <v>12</v>
@@ -1076,7 +1066,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>13</v>
@@ -1084,7 +1074,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
@@ -1093,7 +1083,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>22</v>
@@ -1101,7 +1091,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="6">
         <v>4</v>
@@ -1110,7 +1100,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>14</v>
@@ -1127,7 +1117,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>20</v>
@@ -1144,7 +1134,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>6</v>
@@ -1152,7 +1142,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="6">
         <v>4</v>
@@ -1161,7 +1151,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>17</v>
@@ -1169,7 +1159,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="6">
         <v>4</v>
@@ -1178,7 +1168,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>16</v>
@@ -1186,7 +1176,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="6">
         <v>4</v>
@@ -1195,7 +1185,7 @@
         <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>24</v>
@@ -1203,7 +1193,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="6">
         <v>2</v>
@@ -1212,7 +1202,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="9"/>
     </row>
@@ -1227,7 +1217,7 @@
         <v>54</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>55</v>
@@ -1244,7 +1234,7 @@
         <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>47</v>
@@ -1261,7 +1251,7 @@
         <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>43</v>
@@ -1269,7 +1259,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="6">
         <v>2</v>
@@ -1278,7 +1268,7 @@
         <v>49</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>50</v>
@@ -1286,7 +1276,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="6">
         <v>9</v>
@@ -1295,7 +1285,7 @@
         <v>44</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>45</v>
@@ -1303,7 +1293,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="6">
         <v>8</v>
@@ -1312,7 +1302,7 @@
         <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>41</v>
@@ -1320,7 +1310,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="6">
         <v>2</v>
@@ -1329,7 +1319,7 @@
         <v>51</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>52</v>
@@ -1337,7 +1327,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="6">
         <v>2</v>
@@ -1346,7 +1336,7 @@
         <v>59</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>60</v>
@@ -1363,7 +1353,7 @@
         <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>58</v>
@@ -1371,7 +1361,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="6">
         <v>2</v>
@@ -1380,7 +1370,7 @@
         <v>61</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>62</v>
@@ -1388,16 +1378,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>39</v>
@@ -1405,7 +1395,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="6">
         <v>8</v>
@@ -1414,7 +1404,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>29</v>
@@ -1422,7 +1412,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="6">
         <v>4</v>
@@ -1431,7 +1421,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>28</v>
@@ -1448,7 +1438,7 @@
         <v>27</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>33</v>
@@ -1465,10 +1455,10 @@
         <v>26</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1482,11 +1472,11 @@
         <v>31</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1489,7 @@
       <c r="D33" s="7"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1510,13 +1500,13 @@
         <v>37</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -1527,15 +1517,15 @@
         <v>64</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36" s="6">
         <v>2</v>
@@ -1544,13 +1534,13 @@
         <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -1561,15 +1551,15 @@
         <v>67</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="6">
         <v>2</v>
@@ -1578,35 +1568,32 @@
         <v>68</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="6">
         <v>2</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="E39" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" s="6">
         <v>2</v>
@@ -1618,10 +1605,10 @@
         <v>70</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
@@ -1632,13 +1619,13 @@
         <v>72</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
@@ -1652,12 +1639,12 @@
         <v>74</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="6">
         <v>2</v>
@@ -1666,15 +1653,15 @@
         <v>75</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B44" s="6">
         <v>2</v>
@@ -1683,13 +1670,13 @@
         <v>76</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>77</v>
       </c>
@@ -1700,13 +1687,13 @@
         <v>78</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
@@ -1720,10 +1707,10 @@
         <v>80</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>81</v>
       </c>
@@ -1734,19 +1721,19 @@
         <v>82</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B48" s="5">
         <f>SUM(B17:B47)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C48" s="3"/>
     </row>
@@ -1760,13 +1747,7 @@
       <c r="B51" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1">
-    <filterColumn colId="1"/>
-    <filterColumn colId="4"/>
-    <sortState ref="A2:H239">
-      <sortCondition ref="G1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mostly just a commit so I have a back up of my work. Continued progress on next revision of hardware.
</commit_message>
<xml_diff>
--- a/Hardware/PSDR1_BOM.xlsx
+++ b/Hardware/PSDR1_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="189">
   <si>
     <t>CSM-X7R-100N-10P-25V-0603</t>
   </si>
@@ -544,6 +544,48 @@
   </si>
   <si>
     <t>AD8131ARMZ-ND</t>
+  </si>
+  <si>
+    <t>IC TOUCH SENSOR 1KEY SOT23-6</t>
+  </si>
+  <si>
+    <t>AT42QT1011-TSHR</t>
+  </si>
+  <si>
+    <t>AT42QT1011-TSHRCT-ND</t>
+  </si>
+  <si>
+    <t>Atmel</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2.2nF Cap</t>
+  </si>
+  <si>
+    <t>22k RES</t>
+  </si>
+  <si>
+    <t>100nF Cap</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>CONN HEADER PH SIDE 2POS 2MM</t>
+  </si>
+  <si>
+    <t>455-1719-ND</t>
+  </si>
+  <si>
+    <t>IC MCU ARM 2MB FLASH 100LQFP</t>
+  </si>
+  <si>
+    <t>STM32F429VIT6</t>
+  </si>
+  <si>
+    <t>497-14052-ND</t>
   </si>
 </sst>
 </file>
@@ -911,12 +953,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A49" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C28:C30"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1737,14 +1779,80 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:6">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="2:6">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:6">
       <c r="B51" s="4"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" t="s">
+        <v>184</v>
+      </c>
+      <c r="E56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>

</xml_diff>

<commit_message>
Saving progress. Nothing to see here. Updates to schematic and BOM.
</commit_message>
<xml_diff>
--- a/Hardware/PSDR1_BOM.xlsx
+++ b/Hardware/PSDR1_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="15150" windowHeight="7380"/>
+    <workbookView xWindow="12090" yWindow="285" windowWidth="3060" windowHeight="4500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="202">
   <si>
     <t>CSM-X7R-100N-10P-25V-0603</t>
   </si>
@@ -586,6 +586,45 @@
   </si>
   <si>
     <t>497-14052-ND</t>
+  </si>
+  <si>
+    <t>CONN AUDIO JACK 3.5MM 4COND SMD</t>
+  </si>
+  <si>
+    <t>SJ-43516-SMT-TR</t>
+  </si>
+  <si>
+    <t>CP-43516SJCT-ND</t>
+  </si>
+  <si>
+    <t>CONN JACK 3.5MM R/A 4POS MID SMD</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>SJ-43617-SMT-TR</t>
+  </si>
+  <si>
+    <t>CP-43617SJCT-ND</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.3A SOT23-5</t>
+  </si>
+  <si>
+    <t>MCP1802T-3302I/OT</t>
+  </si>
+  <si>
+    <t>MCP1802T-3302I/OTCT-ND</t>
+  </si>
+  <si>
+    <t>IC POT DGTL 256-TAP 10UMAX</t>
+  </si>
+  <si>
+    <t>MAX5388NAUB+</t>
+  </si>
+  <si>
+    <t>MAX5388NAUB+-ND</t>
   </si>
 </sst>
 </file>
@@ -953,12 +992,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A49" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1852,6 +1891,62 @@
       </c>
       <c r="E57" s="1" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tones of progress on the schematic. I'm getting close!
</commit_message>
<xml_diff>
--- a/Hardware/PSDR1_BOM.xlsx
+++ b/Hardware/PSDR1_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="285" windowWidth="3060" windowHeight="4500"/>
+    <workbookView xWindow="0" yWindow="285" windowWidth="3060" windowHeight="4500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="221">
   <si>
     <t>CSM-X7R-100N-10P-25V-0603</t>
   </si>
@@ -625,6 +625,63 @@
   </si>
   <si>
     <t>MAX5388NAUB+-ND</t>
+  </si>
+  <si>
+    <t>DPDT LEAD FREE SWITCH DC - 6GHZ</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>MASWSS0129TR-3000</t>
+  </si>
+  <si>
+    <t>1465-1374-1-ND</t>
+  </si>
+  <si>
+    <t>watts</t>
+  </si>
+  <si>
+    <t>IC AMP AUDIO PWR 1W MONO 10MSOP</t>
+  </si>
+  <si>
+    <t>TPA0253DGQR</t>
+  </si>
+  <si>
+    <t>296-7006-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 220UF 6.3V 20% X5R 1210</t>
+  </si>
+  <si>
+    <t>1276-3375-1-ND</t>
+  </si>
+  <si>
+    <t>IC SWITCH SPDT SC70-6</t>
+  </si>
+  <si>
+    <t>296-14909-1-ND</t>
+  </si>
+  <si>
+    <t>IC MULTIPLEXER 2X2 10UMAX</t>
+  </si>
+  <si>
+    <t>MAX4525CUB+-ND</t>
+  </si>
+  <si>
+    <t>IC REG BUCK SYNC ADJ 1A SOT25</t>
+  </si>
+  <si>
+    <t>AP3417CKTR-G1DICT-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR 2.2UH 4.2A 30% SMD</t>
+  </si>
+  <si>
+    <t>These are so cheap and small, what's the catch?</t>
+  </si>
+  <si>
+    <t>587-2098-1-ND</t>
   </si>
 </sst>
 </file>
@@ -992,12 +1049,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A49" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1818,16 +1875,16 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:11">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:11">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:11">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:11">
       <c r="B52" s="1" t="s">
         <v>179</v>
       </c>
@@ -1844,7 +1901,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:11">
       <c r="B53" s="1" t="s">
         <v>179</v>
       </c>
@@ -1852,7 +1909,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:11">
       <c r="B54" s="1" t="s">
         <v>179</v>
       </c>
@@ -1860,7 +1917,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:11">
       <c r="B55" s="1" t="s">
         <v>179</v>
       </c>
@@ -1868,7 +1925,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:11">
       <c r="B56" s="1" t="s">
         <v>183</v>
       </c>
@@ -1879,7 +1936,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:11">
       <c r="B57" s="1" t="s">
         <v>183</v>
       </c>
@@ -1893,7 +1950,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:11">
       <c r="B58" s="1" t="s">
         <v>193</v>
       </c>
@@ -1906,8 +1963,15 @@
       <c r="E58" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="59" spans="2:6">
+      <c r="J58">
+        <f>2.6*(0.09+0.04)</f>
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="K58" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11">
       <c r="B59" s="1" t="s">
         <v>183</v>
       </c>
@@ -1921,7 +1985,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:11">
       <c r="B60" s="1" t="s">
         <v>183</v>
       </c>
@@ -1934,8 +1998,11 @@
       <c r="E60" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="61" spans="2:6">
+      <c r="K60">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11">
       <c r="B61" s="1" t="s">
         <v>183</v>
       </c>
@@ -1947,6 +2014,104 @@
       </c>
       <c r="E61" s="1" t="s">
         <v>201</v>
+      </c>
+      <c r="K61">
+        <f>K60/(90+40)</f>
+        <v>15.384615384615385</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11">
+      <c r="B62" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="B63" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="B64" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11">
+      <c r="B65" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K65">
+        <f>2.9*0.15</f>
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11">
+      <c r="B66" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K66">
+        <f>2000/150</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="B68" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More progress on PSDR2. Schematic is basically complete (at least, all the components and blocks are in, though some connections between blocks and to the MCU are not in there yet.) Also started layout. Location sensitive components have been placed. It's going to be so cool!
</commit_message>
<xml_diff>
--- a/Hardware/PSDR1_BOM.xlsx
+++ b/Hardware/PSDR1_BOM.xlsx
@@ -1051,10 +1051,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A49" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
PSDR2 Release. Schematic, layout, and gerbers complete. PSDR1 gerbers moved to Old folder (probably should just call it PSDR1...) Started (and almost finished) Encoder daughterboard.
</commit_message>
<xml_diff>
--- a/Hardware/PSDR1_BOM.xlsx
+++ b/Hardware/PSDR1_BOM.xlsx
@@ -1052,9 +1052,9 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A49" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A40" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>